<commit_message>
Changing forms to test data type checks
</commit_message>
<xml_diff>
--- a/test/sample_forms/Form-1RC.xlsx
+++ b/test/sample_forms/Form-1RC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\base\forms\base-form-management\test\test_forms\old\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\R libs\base\forms\base-form-management\test\sample_forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79F245F-91E8-4FA2-B889-05511BFD8278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C2A406-1DE5-4D4E-9F84-D6858793997A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="5O4euoXp3wZfikUhVbwGMfw3acpHwF0QGHqLGhqkSE4QfnoccY7VPEsDDzzEBP5NB49UT+XbcZf1lZQTbDpLFA==" workbookSaltValue="DtEOIJKZ9UKP8oWrD+QpRw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1140" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="90">
   <si>
     <t>Focal point</t>
   </si>
@@ -301,6 +301,12 @@
   </si>
   <si>
     <t>HL-FS[IN]SW</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>UN</t>
   </si>
 </sst>
 </file>
@@ -1636,7 +1642,7 @@
       <pane xSplit="10" ySplit="5" topLeftCell="K6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2411,7 +2417,7 @@
         <v>36</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>39</v>
@@ -3200,7 +3206,7 @@
         <v>36</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="G13" s="29" t="s">
         <v>39</v>
@@ -3462,7 +3468,7 @@
         <v>36</v>
       </c>
       <c r="F15" s="28" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="G15" s="29" t="s">
         <v>39</v>
@@ -4492,7 +4498,7 @@
         <v>36</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>42</v>
+        <v>88</v>
       </c>
       <c r="G23" s="29" t="s">
         <v>43</v>

</xml_diff>